<commit_message>
Error handling added on Excel
</commit_message>
<xml_diff>
--- a/Data/ConfigFile.xlsx
+++ b/Data/ConfigFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dee\Documents\UiPath\Assignment1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14390F74-2706-47F5-9CA5-19F77BADF577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6EF57C-C1FC-45C7-B70D-884862EF578C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="1860" windowWidth="21600" windowHeight="7575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>https://www.mobile.de/ro/automobil/mazda-cx-5/vhc:car,cnt:de,ms1:16800_33_,frn:2012,frx:2018,ful:diesel!electricity,mlx:100000,vcg:</t>
+  </si>
+  <si>
+    <t>https://www.mobile.de/ro/automobil/mazda-cx-5/vhc:car,cnt:de,pgn:1,pgs:50,ms1:16800_33_,frn:2012,frx:2018,ful:diesel!electricity,mlx:100000</t>
   </si>
 </sst>
 </file>
@@ -389,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,7 +405,7 @@
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -413,23 +416,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{CAE187B7-AF37-4726-A40A-C94C73AE79C1}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{CAE187B7-AF37-4726-A40A-C94C73AE79C1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Email activities using config file and text file for email body
</commit_message>
<xml_diff>
--- a/Data/ConfigFile.xlsx
+++ b/Data/ConfigFile.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dee\Documents\UiPath\Assignment1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6EF57C-C1FC-45C7-B70D-884862EF578C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA868BE-8E67-443B-9041-C071B6482696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
+    <sheet name="Email" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -48,13 +49,28 @@
     <t>url</t>
   </si>
   <si>
-    <t>url for the filtered data</t>
-  </si>
-  <si>
-    <t>https://www.mobile.de/ro/automobil/mazda-cx-5/vhc:car,cnt:de,ms1:16800_33_,frn:2012,frx:2018,ful:diesel!electricity,mlx:100000,vcg:</t>
-  </si>
-  <si>
     <t>https://www.mobile.de/ro/automobil/mazda-cx-5/vhc:car,cnt:de,pgn:1,pgs:50,ms1:16800_33_,frn:2012,frx:2018,ful:diesel!electricity,mlx:100000</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>diana.gradinaru.sincai@gmail.com</t>
+  </si>
+  <si>
+    <t>Email address</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>Email subject</t>
+  </si>
+  <si>
+    <t>Assignment number 1 done</t>
+  </si>
+  <si>
+    <t>url for the filtered data, 50 results per page</t>
   </si>
 </sst>
 </file>
@@ -107,10 +123,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -395,7 +414,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,23 +440,75 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{CAE187B7-AF37-4726-A40A-C94C73AE79C1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADD43EC-9947-47E2-8150-AA358E36B9C1}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Email address in config file updated
</commit_message>
<xml_diff>
--- a/Data/ConfigFile.xlsx
+++ b/Data/ConfigFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dee\Documents\UiPath\Assignment1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA868BE-8E67-443B-9041-C071B6482696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2E5C7D-5BF3-4A2E-B86D-D0F7F359EB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>diana.gradinaru.sincai@gmail.com</t>
-  </si>
-  <si>
     <t>Email address</t>
   </si>
   <si>
@@ -71,6 +68,9 @@
   </si>
   <si>
     <t>url for the filtered data, 50 results per page</t>
+  </si>
+  <si>
+    <t>delia.panca@fwfcompany.com</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -443,7 +443,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADD43EC-9947-47E2-8150-AA358E36B9C1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,29 +486,32 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6C19BC26-D8B6-4DE8-8B3D-229A4D695CC2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>